<commit_message>
Fix empty AOQ done list that displays error
</commit_message>
<xml_diff>
--- a/item_details.xlsx
+++ b/item_details.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>ITEM DETAILS</t>
   </si>
@@ -23,22 +23,25 @@
     <t>Item Name:</t>
   </si>
   <si>
-    <t>Acetylene</t>
+    <t>Y-Strainer</t>
   </si>
   <si>
     <t>Brand:</t>
   </si>
   <si>
+    <t>Ever</t>
+  </si>
+  <si>
+    <t>Specifications:</t>
+  </si>
+  <si>
+    <t>150 lbs Rating, Flange Type, Cast Iron, 8"</t>
+  </si>
+  <si>
+    <t>Part Number:</t>
+  </si>
+  <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>Specifications:</t>
-  </si>
-  <si>
-    <t>Refill</t>
-  </si>
-  <si>
-    <t>Part Number:</t>
   </si>
   <si>
     <t>VENDOR LIST</t>
@@ -510,12 +513,12 @@
         <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -528,31 +531,31 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>